<commit_message>
modified benchmarks for modular measurement
</commit_message>
<xml_diff>
--- a/benchmark-harness/comparison/bench.findbugs.reread-memory.xlsx
+++ b/benchmark-harness/comparison/bench.findbugs.reread-memory.xlsx
@@ -136,7 +136,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -620,7 +620,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>0.128</v>
       </c>
       <c r="H2" s="3">
-        <f>E2/N2</f>
+        <f t="shared" ref="H2:H26" si="0">E2/N2</f>
         <v>7.9528907922912211E-3</v>
       </c>
       <c r="I2">
@@ -1067,7 +1067,7 @@
         <v>0.112</v>
       </c>
       <c r="M2" s="3">
-        <f>J2/O2</f>
+        <f t="shared" ref="M2:M26" si="1">J2/O2</f>
         <v>1.4183783783783785E-2</v>
       </c>
       <c r="N2">
@@ -1103,7 +1103,7 @@
         <v>0.17</v>
       </c>
       <c r="H3" s="3">
-        <f>E3/N3</f>
+        <f t="shared" si="0"/>
         <v>4.3276231263383296E-3</v>
       </c>
       <c r="I3">
@@ -1119,7 +1119,7 @@
         <v>0.109</v>
       </c>
       <c r="M3" s="3">
-        <f>J3/O3</f>
+        <f t="shared" si="1"/>
         <v>1.3675675675675675E-2</v>
       </c>
       <c r="N3">
@@ -1155,7 +1155,7 @@
         <v>0.14399999999999999</v>
       </c>
       <c r="H4" s="3">
-        <f>E4/N4</f>
+        <f t="shared" si="0"/>
         <v>3.6680942184154179E-3</v>
       </c>
       <c r="I4">
@@ -1171,7 +1171,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="M4" s="3">
-        <f>J4/O4</f>
+        <f t="shared" si="1"/>
         <v>1.2054054054054054E-2</v>
       </c>
       <c r="N4">
@@ -1207,7 +1207,7 @@
         <v>0.125</v>
       </c>
       <c r="H5" s="3">
-        <f>E5/N5</f>
+        <f t="shared" si="0"/>
         <v>3.1820128479657385E-3</v>
       </c>
       <c r="I5">
@@ -1223,7 +1223,7 @@
         <v>0.109</v>
       </c>
       <c r="M5" s="3">
-        <f>J5/O5</f>
+        <f t="shared" si="1"/>
         <v>1.132972972972973E-2</v>
       </c>
       <c r="N5">
@@ -1259,7 +1259,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="H6" s="3">
-        <f>E6/N6</f>
+        <f t="shared" si="0"/>
         <v>0.1066423982869379</v>
       </c>
       <c r="I6">
@@ -1275,7 +1275,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="M6" s="3">
-        <f>J6/O6</f>
+        <f t="shared" si="1"/>
         <v>0.10673513513513513</v>
       </c>
       <c r="N6">
@@ -1311,7 +1311,7 @@
         <v>0.06</v>
       </c>
       <c r="H7" s="3">
-        <f>E7/N7</f>
+        <f t="shared" si="0"/>
         <v>2.7852248394004284E-2</v>
       </c>
       <c r="I7">
@@ -1327,7 +1327,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="M7" s="3">
-        <f>J7/O7</f>
+        <f t="shared" si="1"/>
         <v>6.0075675675675677E-2</v>
       </c>
       <c r="N7">
@@ -1363,7 +1363,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="H8" s="3">
-        <f>E8/N8</f>
+        <f t="shared" si="0"/>
         <v>1.9316916488222698E-2</v>
       </c>
       <c r="I8">
@@ -1379,7 +1379,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="M8" s="3">
-        <f>J8/O8</f>
+        <f t="shared" si="1"/>
         <v>4.8302702702702704E-2</v>
       </c>
       <c r="N8">
@@ -1415,7 +1415,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="H9" s="3">
-        <f>E9/N9</f>
+        <f t="shared" si="0"/>
         <v>5.0578158458244114E-2</v>
       </c>
       <c r="I9">
@@ -1431,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="3">
-        <f>J9/O9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N9">
@@ -1464,7 +1464,7 @@
         <v>0.13</v>
       </c>
       <c r="H10" s="3">
-        <f>E10/N10</f>
+        <f t="shared" si="0"/>
         <v>3.3040685224839401E-3</v>
       </c>
       <c r="I10">
@@ -1480,7 +1480,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="M10" s="3">
-        <f>J10/O10</f>
+        <f t="shared" si="1"/>
         <v>1.2972972972972972E-2</v>
       </c>
       <c r="N10">
@@ -1516,7 +1516,7 @@
         <v>0.124</v>
       </c>
       <c r="H11" s="3">
-        <f>E11/N11</f>
+        <f t="shared" si="0"/>
         <v>1.6531049250535331E-2</v>
       </c>
       <c r="I11">
@@ -1532,7 +1532,7 @@
         <v>0.104</v>
       </c>
       <c r="M11" s="3">
-        <f>J11/O11</f>
+        <f t="shared" si="1"/>
         <v>1.3027027027027028E-2</v>
       </c>
       <c r="N11">
@@ -1568,7 +1568,7 @@
         <v>0.104</v>
       </c>
       <c r="H12" s="3">
-        <f>E12/N12</f>
+        <f t="shared" si="0"/>
         <v>0.10656102783725911</v>
       </c>
       <c r="I12">
@@ -1584,7 +1584,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M12" s="3">
-        <f>J12/O12</f>
+        <f t="shared" si="1"/>
         <v>0.13378378378378378</v>
       </c>
       <c r="N12">
@@ -1620,7 +1620,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H13" s="3">
-        <f>E13/N13</f>
+        <f t="shared" si="0"/>
         <v>1.3276231263383297E-4</v>
       </c>
       <c r="I13">
@@ -1636,7 +1636,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="M13" s="3">
-        <f>J13/O13</f>
+        <f t="shared" si="1"/>
         <v>1.1091891891891891E-2</v>
       </c>
       <c r="N13">
@@ -1672,7 +1672,7 @@
         <v>0.06</v>
       </c>
       <c r="H14" s="3">
-        <f>E14/N14</f>
+        <f t="shared" si="0"/>
         <v>2.753104925053533E-2</v>
       </c>
       <c r="I14">
@@ -1688,7 +1688,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="M14" s="3">
-        <f>J14/O14</f>
+        <f t="shared" si="1"/>
         <v>6.2810810810810802E-2</v>
       </c>
       <c r="N14">
@@ -1724,7 +1724,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H15" s="3">
-        <f>E15/N15</f>
+        <f t="shared" si="0"/>
         <v>1.2205567451820129E-4</v>
       </c>
       <c r="I15">
@@ -1740,7 +1740,7 @@
         <v>0.1</v>
       </c>
       <c r="M15" s="3">
-        <f>J15/O15</f>
+        <f t="shared" si="1"/>
         <v>1.2562162162162162E-2</v>
       </c>
       <c r="N15">
@@ -1776,7 +1776,7 @@
         <v>0.06</v>
       </c>
       <c r="H16" s="3">
-        <f>E16/N16</f>
+        <f t="shared" si="0"/>
         <v>2.7629550321199143E-2</v>
       </c>
       <c r="I16">
@@ -1792,7 +1792,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="M16" s="3">
-        <f>J16/O16</f>
+        <f t="shared" si="1"/>
         <v>6.2800000000000009E-2</v>
       </c>
       <c r="N16">
@@ -1828,7 +1828,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="H17" s="3">
-        <f>E17/N17</f>
+        <f t="shared" si="0"/>
         <v>2.7201284796573875E-2</v>
       </c>
       <c r="I17">
@@ -1844,7 +1844,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M17" s="3">
-        <f>J17/O17</f>
+        <f t="shared" si="1"/>
         <v>6.2551351351351342E-2</v>
       </c>
       <c r="N17">
@@ -1880,7 +1880,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="H18" s="3">
-        <f>E18/N18</f>
+        <f t="shared" si="0"/>
         <v>2.7256959314775158E-2</v>
       </c>
       <c r="I18">
@@ -1896,7 +1896,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="M18" s="3">
-        <f>J18/O18</f>
+        <f t="shared" si="1"/>
         <v>6.2616216216216214E-2</v>
       </c>
       <c r="N18">
@@ -1932,7 +1932,7 @@
         <v>0.01</v>
       </c>
       <c r="H19" s="3">
-        <f>E19/N19</f>
+        <f t="shared" si="0"/>
         <v>7.7087794432548177E-5</v>
       </c>
       <c r="I19">
@@ -1948,7 +1948,7 @@
         <v>0.107</v>
       </c>
       <c r="M19" s="3">
-        <f>J19/O19</f>
+        <f t="shared" si="1"/>
         <v>1.2670270270270269E-2</v>
       </c>
       <c r="N19">
@@ -1984,7 +1984,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H20" s="3">
-        <f>E20/N20</f>
+        <f t="shared" si="0"/>
         <v>5.9957173447537476E-5</v>
       </c>
       <c r="I20">
@@ -2000,7 +2000,7 @@
         <v>0.106</v>
       </c>
       <c r="M20" s="3">
-        <f>J20/O20</f>
+        <f t="shared" si="1"/>
         <v>1.2054054054054054E-2</v>
       </c>
       <c r="N20">
@@ -2036,7 +2036,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H21" s="3">
-        <f>E21/N21</f>
+        <f t="shared" si="0"/>
         <v>1.4775160599571737E-4</v>
       </c>
       <c r="I21">
@@ -2052,7 +2052,7 @@
         <v>0.105</v>
       </c>
       <c r="M21" s="3">
-        <f>J21/O21</f>
+        <f t="shared" si="1"/>
         <v>1.2475675675675675E-2</v>
       </c>
       <c r="N21">
@@ -2088,7 +2088,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H22" s="3">
-        <f>E22/N22</f>
+        <f t="shared" si="0"/>
         <v>1.2633832976445395E-4</v>
       </c>
       <c r="I22">
@@ -2104,7 +2104,7 @@
         <v>0.104</v>
       </c>
       <c r="M22" s="3">
-        <f>J22/O22</f>
+        <f t="shared" si="1"/>
         <v>1.184864864864865E-2</v>
       </c>
       <c r="N22">
@@ -2140,7 +2140,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="H23" s="3">
-        <f>E23/N23</f>
+        <f t="shared" si="0"/>
         <v>1.1349036402569593E-4</v>
       </c>
       <c r="I23">
@@ -2156,7 +2156,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="M23" s="3">
-        <f>J23/O23</f>
+        <f t="shared" si="1"/>
         <v>1.1686486486486486E-2</v>
       </c>
       <c r="N23">
@@ -2192,7 +2192,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="H24" s="3">
-        <f>E24/N24</f>
+        <f t="shared" si="0"/>
         <v>1.4955032119914348E-2</v>
       </c>
       <c r="I24">
@@ -2208,7 +2208,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M24" s="3">
-        <f>J24/O24</f>
+        <f t="shared" si="1"/>
         <v>3.3243243243243244E-2</v>
       </c>
       <c r="N24">
@@ -2244,7 +2244,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="H25" s="3">
-        <f>E25/N25</f>
+        <f t="shared" si="0"/>
         <v>4.4608137044967883E-2</v>
       </c>
       <c r="I25">
@@ -2260,7 +2260,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="M25" s="3">
-        <f>J25/O25</f>
+        <f t="shared" si="1"/>
         <v>6.8962162162162152E-2</v>
       </c>
       <c r="N25">
@@ -2293,7 +2293,7 @@
         <v>0.312</v>
       </c>
       <c r="H26" s="3">
-        <f>E26/N26</f>
+        <f t="shared" si="0"/>
         <v>0.26077516059957173</v>
       </c>
       <c r="I26">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="3">
-        <f>J26/O26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N26">

</xml_diff>